<commit_message>
Data for main page from wine.xlsx
</commit_message>
<xml_diff>
--- a/files/wine.xlsx
+++ b/files/wine.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ray\PycharmProjects\devman_frontend_lesson1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ray\PycharmProjects\devman_frontend_lesson1\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,18 +21,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
-    <t>Название</t>
-  </si>
-  <si>
-    <t>Сорт</t>
-  </si>
-  <si>
-    <t>Цена</t>
-  </si>
-  <si>
-    <t>Картинка</t>
-  </si>
-  <si>
     <t>Изабелла</t>
   </si>
   <si>
@@ -76,6 +64,18 @@
   </si>
   <si>
     <t>hvanchkara.png</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>wine_sort</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>picture</t>
   </si>
 </sst>
 </file>
@@ -350,7 +350,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -362,100 +362,100 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C2" s="2">
         <v>350</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C3" s="2">
         <v>350</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C4" s="2">
         <v>350</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C5" s="2">
         <v>399</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C6" s="2">
         <v>499</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C7" s="2">
         <v>550</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>